<commit_message>
update double checking codes
</commit_message>
<xml_diff>
--- a/LCA/LCI_ Inventories.xlsx
+++ b/LCA/LCI_ Inventories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mamy/PAW/PAW_MFA_LCA_2025/LCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FF092F-67DC-CF43-A2AC-FA9A7D1B270C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82A3A1B-D0F5-3142-AE64-A891A0F2315D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33400" yWindow="-140" windowWidth="34640" windowHeight="19480" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
+    <workbookView xWindow="30240" yWindow="-1500" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
   </bookViews>
   <sheets>
     <sheet name="Directory" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="141">
   <si>
     <t>Database</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>treatment of sewage sludge, 70% water, WWT, WW, average, municipal incineration</t>
-  </si>
-  <si>
-    <t>sec_tre</t>
   </si>
   <si>
     <t>secondary treatment</t>
@@ -950,10 +947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9BD897-F590-4437-A121-ED2632AD5485}">
-  <dimension ref="A1:O220"/>
+  <dimension ref="A1:O222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="173" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200"/>
+    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="173" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -977,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1181,7 +1178,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C19">
         <v>0.23100000000000001</v>
@@ -1190,13 +1187,13 @@
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19" t="s">
         <v>42</v>
@@ -1425,7 +1422,7 @@
         <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F35" t="s">
         <v>41</v>
@@ -1472,7 +1469,7 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F36" t="s">
         <v>41</v>
@@ -1707,7 +1704,7 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F52" t="s">
         <v>41</v>
@@ -1754,7 +1751,7 @@
         <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F53" t="s">
         <v>41</v>
@@ -1801,7 +1798,7 @@
         <v>48</v>
       </c>
       <c r="E54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F54" t="s">
         <v>41</v>
@@ -1848,7 +1845,7 @@
         <v>48</v>
       </c>
       <c r="E55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F55" t="s">
         <v>41</v>
@@ -1895,7 +1892,7 @@
         <v>48</v>
       </c>
       <c r="E56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" t="s">
         <v>41</v>
@@ -1942,7 +1939,7 @@
         <v>48</v>
       </c>
       <c r="E57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F57" t="s">
         <v>41</v>
@@ -1989,7 +1986,7 @@
         <v>48</v>
       </c>
       <c r="E58" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F58" t="s">
         <v>41</v>
@@ -2036,7 +2033,7 @@
         <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F59" t="s">
         <v>41</v>
@@ -2083,7 +2080,7 @@
         <v>48</v>
       </c>
       <c r="E60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F60" t="s">
         <v>41</v>
@@ -2130,7 +2127,7 @@
         <v>48</v>
       </c>
       <c r="E61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F61" t="s">
         <v>41</v>
@@ -2177,7 +2174,7 @@
         <v>48</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" t="s">
         <v>41</v>
@@ -2224,7 +2221,7 @@
         <v>48</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F63" t="s">
         <v>41</v>
@@ -2271,7 +2268,7 @@
         <v>48</v>
       </c>
       <c r="E64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F64" t="s">
         <v>41</v>
@@ -2318,7 +2315,7 @@
         <v>48</v>
       </c>
       <c r="E65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F65" t="s">
         <v>41</v>
@@ -2365,7 +2362,7 @@
         <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F66" t="s">
         <v>41</v>
@@ -2412,7 +2409,7 @@
         <v>48</v>
       </c>
       <c r="E67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F67" t="s">
         <v>41</v>
@@ -2459,7 +2456,7 @@
         <v>48</v>
       </c>
       <c r="E68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F68" t="s">
         <v>41</v>
@@ -2506,7 +2503,7 @@
         <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F69" t="s">
         <v>41</v>
@@ -2741,7 +2738,7 @@
         <v>48</v>
       </c>
       <c r="E85" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F85" t="s">
         <v>99</v>
@@ -2788,7 +2785,7 @@
         <v>48</v>
       </c>
       <c r="E86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F86" t="s">
         <v>41</v>
@@ -2835,7 +2832,7 @@
         <v>21</v>
       </c>
       <c r="E87" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F87" t="s">
         <v>41</v>
@@ -2882,7 +2879,7 @@
         <v>48</v>
       </c>
       <c r="E88" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F88" t="s">
         <v>41</v>
@@ -2920,235 +2917,191 @@
         <v>8</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>11</v>
-      </c>
-      <c r="B92">
-        <v>230</v>
+      <c r="A92" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>15</v>
-      </c>
-      <c r="B93" t="s">
-        <v>128</v>
+        <v>11</v>
+      </c>
+      <c r="B93">
+        <v>230</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>17</v>
-      </c>
-      <c r="B94">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B94" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>18</v>
-      </c>
-      <c r="B95" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B97" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B98" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>9</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>25</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>17</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" t="s">
         <v>20</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>26</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F100" t="s">
         <v>27</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G100" t="s">
         <v>15</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H100" t="s">
         <v>18</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I100" t="s">
         <v>22</v>
       </c>
-      <c r="J99" t="s">
+      <c r="J100" t="s">
         <v>28</v>
       </c>
-      <c r="K99" t="s">
+      <c r="K100" t="s">
         <v>29</v>
       </c>
-      <c r="L99" t="s">
+      <c r="L100" t="s">
         <v>30</v>
       </c>
-      <c r="M99" t="s">
+      <c r="M100" t="s">
         <v>31</v>
       </c>
-      <c r="N99" t="s">
+      <c r="N100" t="s">
         <v>32</v>
       </c>
-      <c r="O99" t="s">
+      <c r="O100" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A100" t="str">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" t="str">
         <f>B91</f>
-        <v>sec_tre</v>
-      </c>
-      <c r="B100" t="str">
+        <v>sec_tre__qua_tre</v>
+      </c>
+      <c r="B101" t="str">
         <f>B90</f>
         <v>Activated Carbon Technology</v>
       </c>
-      <c r="C100">
+      <c r="C101">
         <v>1</v>
       </c>
-      <c r="D100" t="str">
-        <f>B96</f>
+      <c r="D101" t="str">
+        <f>B97</f>
         <v>cubic meter</v>
       </c>
-      <c r="E100" t="str">
+      <c r="E101" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F101" t="s">
         <v>34</v>
       </c>
-      <c r="G100" t="str">
-        <f>B93</f>
+      <c r="G101" t="str">
+        <f>B94</f>
         <v>DE</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H101" t="s">
         <v>35</v>
       </c>
-      <c r="I100" t="str">
-        <f>B97</f>
+      <c r="I101" t="str">
+        <f>B98</f>
         <v>wastewater, average</v>
       </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100" t="s">
-        <v>36</v>
-      </c>
-      <c r="L100" t="s">
-        <v>36</v>
-      </c>
-      <c r="M100" t="s">
-        <v>36</v>
-      </c>
-      <c r="N100" t="s">
-        <v>36</v>
-      </c>
-      <c r="O100" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>36</v>
-      </c>
-      <c r="B101" t="str">
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101" t="s">
+        <v>36</v>
+      </c>
+      <c r="L101" t="s">
+        <v>36</v>
+      </c>
+      <c r="M101" t="s">
+        <v>36</v>
+      </c>
+      <c r="N101" t="s">
+        <v>36</v>
+      </c>
+      <c r="O101" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" t="str">
         <f>B71</f>
         <v>Emissions 230</v>
       </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-      <c r="D101" t="str">
-        <f>B80</f>
-        <v>cubic meter</v>
-      </c>
-      <c r="E101" t="str">
-        <f>E100</f>
-        <v>paw_db</v>
-      </c>
-      <c r="F101" t="s">
-        <v>41</v>
-      </c>
-      <c r="G101" t="str">
-        <f>B77</f>
-        <v>RER</v>
-      </c>
-      <c r="H101" t="s">
-        <v>42</v>
-      </c>
-      <c r="I101" t="str">
-        <f>B81</f>
-        <v>direct emissions per m3</v>
-      </c>
-      <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101" t="s">
-        <v>36</v>
-      </c>
-      <c r="L101" t="s">
-        <v>36</v>
-      </c>
-      <c r="M101" t="s">
-        <v>36</v>
-      </c>
-      <c r="N101" t="s">
-        <v>36</v>
-      </c>
-      <c r="O101" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>36</v>
-      </c>
-      <c r="B102" t="str">
-        <f>B38</f>
-        <v>Chemicals 230</v>
-      </c>
       <c r="C102">
         <v>1</v>
       </c>
       <c r="D102" t="str">
-        <f>B47</f>
+        <f>B80</f>
         <v>cubic meter</v>
       </c>
       <c r="E102" t="str">
@@ -3156,21 +3109,21 @@
         <v>paw_db</v>
       </c>
       <c r="F102" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G102" t="str">
-        <f>B44</f>
+        <f>B77</f>
         <v>RER</v>
       </c>
       <c r="H102" t="s">
         <v>42</v>
       </c>
       <c r="I102" t="str">
-        <f>B48</f>
-        <v>chemicals per m3</v>
+        <f>B81</f>
+        <v>direct emissions per m3</v>
       </c>
       <c r="J102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K102" t="s">
         <v>36</v>
@@ -3193,14 +3146,14 @@
         <v>36</v>
       </c>
       <c r="B103" t="str">
-        <f>B21</f>
-        <v>GAC 230</v>
+        <f>B38</f>
+        <v>Chemicals 230</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
       <c r="D103" t="str">
-        <f>B30</f>
+        <f>B47</f>
         <v>cubic meter</v>
       </c>
       <c r="E103" t="str">
@@ -3211,18 +3164,18 @@
         <v>34</v>
       </c>
       <c r="G103" t="str">
-        <f>B27</f>
+        <f>B44</f>
         <v>RER</v>
       </c>
       <c r="H103" t="s">
         <v>42</v>
       </c>
       <c r="I103" t="str">
-        <f>B31</f>
-        <v>GAC per m3</v>
+        <f>B48</f>
+        <v>chemicals per m3</v>
       </c>
       <c r="J103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K103" t="s">
         <v>36</v>
@@ -3245,14 +3198,14 @@
         <v>36</v>
       </c>
       <c r="B104" t="str">
-        <f>B5</f>
-        <v>Electricity 230</v>
+        <f>B21</f>
+        <v>GAC 230</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
       <c r="D104" t="str">
-        <f>B14</f>
+        <f>B30</f>
         <v>cubic meter</v>
       </c>
       <c r="E104" t="str">
@@ -3263,474 +3216,479 @@
         <v>34</v>
       </c>
       <c r="G104" t="str">
+        <f>B27</f>
+        <v>RER</v>
+      </c>
+      <c r="H104" t="s">
+        <v>42</v>
+      </c>
+      <c r="I104" t="str">
+        <f>B31</f>
+        <v>GAC per m3</v>
+      </c>
+      <c r="J104">
+        <v>2</v>
+      </c>
+      <c r="K104" t="s">
+        <v>36</v>
+      </c>
+      <c r="L104" t="s">
+        <v>36</v>
+      </c>
+      <c r="M104" t="s">
+        <v>36</v>
+      </c>
+      <c r="N104" t="s">
+        <v>36</v>
+      </c>
+      <c r="O104" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>36</v>
+      </c>
+      <c r="B105" t="str">
+        <f>B5</f>
+        <v>Electricity 230</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="str">
+        <f>B14</f>
+        <v>cubic meter</v>
+      </c>
+      <c r="E105" t="str">
+        <f>E104</f>
+        <v>paw_db</v>
+      </c>
+      <c r="F105" t="s">
+        <v>34</v>
+      </c>
+      <c r="G105" t="str">
         <f>B11</f>
         <v>RER</v>
       </c>
-      <c r="H104" t="s">
+      <c r="H105" t="s">
         <v>42</v>
       </c>
-      <c r="I104" t="str">
+      <c r="I105" t="str">
         <f>B15</f>
         <v>electricity per m3</v>
       </c>
-      <c r="J104">
+      <c r="J105">
         <v>3</v>
       </c>
-      <c r="K104" t="s">
-        <v>36</v>
-      </c>
-      <c r="L104" t="s">
-        <v>36</v>
-      </c>
-      <c r="M104" t="s">
-        <v>36</v>
-      </c>
-      <c r="N104" t="s">
-        <v>36</v>
-      </c>
-      <c r="O104" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="K105" t="s">
+        <v>36</v>
+      </c>
+      <c r="L105" t="s">
+        <v>36</v>
+      </c>
+      <c r="M105" t="s">
+        <v>36</v>
+      </c>
+      <c r="N105" t="s">
+        <v>36</v>
+      </c>
+      <c r="O105" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>9</v>
-      </c>
-      <c r="B107" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
-      </c>
-      <c r="B109">
-        <v>102</v>
+        <v>10</v>
+      </c>
+      <c r="B109" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>12</v>
-      </c>
-      <c r="B110" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B110">
+        <v>102</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B112" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>17</v>
-      </c>
-      <c r="B113">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B113" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>18</v>
-      </c>
-      <c r="B114" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B115" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B116" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" t="s">
-        <v>25</v>
-      </c>
-      <c r="C118" t="s">
-        <v>17</v>
-      </c>
-      <c r="D118" t="s">
-        <v>20</v>
-      </c>
-      <c r="E118" t="s">
-        <v>26</v>
-      </c>
-      <c r="F118" t="s">
-        <v>27</v>
-      </c>
-      <c r="G118" t="s">
-        <v>15</v>
-      </c>
-      <c r="H118" t="s">
-        <v>18</v>
-      </c>
-      <c r="I118" t="s">
-        <v>22</v>
-      </c>
-      <c r="J118" t="s">
-        <v>28</v>
-      </c>
-      <c r="K118" t="s">
-        <v>29</v>
-      </c>
-      <c r="L118" t="s">
-        <v>30</v>
-      </c>
-      <c r="M118" t="s">
-        <v>31</v>
-      </c>
-      <c r="N118" t="s">
-        <v>32</v>
-      </c>
-      <c r="O118" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D119" t="s">
+        <v>20</v>
+      </c>
+      <c r="E119" t="s">
+        <v>26</v>
+      </c>
+      <c r="F119" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" t="s">
+        <v>15</v>
+      </c>
+      <c r="H119" t="s">
+        <v>18</v>
+      </c>
+      <c r="I119" t="s">
+        <v>22</v>
+      </c>
+      <c r="J119" t="s">
+        <v>28</v>
+      </c>
+      <c r="K119" t="s">
+        <v>29</v>
+      </c>
+      <c r="L119" t="s">
+        <v>30</v>
+      </c>
+      <c r="M119" t="s">
+        <v>31</v>
+      </c>
+      <c r="N119" t="s">
+        <v>32</v>
+      </c>
+      <c r="O119" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>105</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>104</v>
       </c>
-      <c r="C119">
+      <c r="C120">
         <v>1</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>21</v>
       </c>
-      <c r="E119" t="str">
+      <c r="E120" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F119" t="s">
-        <v>34</v>
-      </c>
-      <c r="G119" t="s">
-        <v>16</v>
-      </c>
-      <c r="H119" t="s">
-        <v>35</v>
-      </c>
-      <c r="I119" t="s">
-        <v>23</v>
-      </c>
-      <c r="J119">
-        <v>0</v>
-      </c>
-      <c r="K119" t="s">
-        <v>36</v>
-      </c>
-      <c r="L119" t="s">
-        <v>36</v>
-      </c>
-      <c r="M119" t="s">
-        <v>36</v>
-      </c>
-      <c r="N119" t="s">
-        <v>36</v>
-      </c>
-      <c r="O119" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>36</v>
-      </c>
-      <c r="B120" t="s">
-        <v>132</v>
-      </c>
-      <c r="C120">
-        <v>0.17</v>
-      </c>
-      <c r="D120" t="s">
-        <v>40</v>
-      </c>
-      <c r="E120" t="s">
-        <v>124</v>
-      </c>
       <c r="F120" t="s">
         <v>34</v>
       </c>
       <c r="G120" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="H120" t="s">
+        <v>35</v>
+      </c>
+      <c r="I120" t="s">
+        <v>23</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120" t="s">
+        <v>36</v>
+      </c>
+      <c r="L120" t="s">
+        <v>36</v>
+      </c>
+      <c r="M120" t="s">
+        <v>36</v>
+      </c>
+      <c r="N120" t="s">
+        <v>36</v>
+      </c>
+      <c r="O120" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>36</v>
+      </c>
+      <c r="B121" t="s">
+        <v>131</v>
+      </c>
+      <c r="C121">
+        <v>0.17</v>
+      </c>
+      <c r="D121" t="s">
+        <v>40</v>
+      </c>
+      <c r="E121" t="s">
+        <v>123</v>
+      </c>
+      <c r="F121" t="s">
+        <v>34</v>
+      </c>
+      <c r="G121" t="s">
+        <v>127</v>
+      </c>
+      <c r="H121" t="s">
         <v>42</v>
       </c>
-      <c r="I120" t="s">
+      <c r="I121" t="s">
         <v>43</v>
       </c>
-      <c r="J120">
-        <v>0</v>
-      </c>
-      <c r="K120" t="s">
-        <v>36</v>
-      </c>
-      <c r="L120" t="s">
-        <v>36</v>
-      </c>
-      <c r="M120" t="s">
-        <v>36</v>
-      </c>
-      <c r="N120" t="s">
-        <v>36</v>
-      </c>
-      <c r="O120" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121" t="s">
+        <v>36</v>
+      </c>
+      <c r="L121" t="s">
+        <v>36</v>
+      </c>
+      <c r="M121" t="s">
+        <v>36</v>
+      </c>
+      <c r="N121" t="s">
+        <v>36</v>
+      </c>
+      <c r="O121" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
-      </c>
-      <c r="B125">
-        <v>102</v>
+        <v>10</v>
+      </c>
+      <c r="B125" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>12</v>
-      </c>
-      <c r="B126" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B126">
+        <v>102</v>
       </c>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>17</v>
-      </c>
-      <c r="B129">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B129" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>18</v>
-      </c>
-      <c r="B130" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B131" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B132" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B133" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>9</v>
-      </c>
-      <c r="B134" t="s">
-        <v>25</v>
-      </c>
-      <c r="C134" t="s">
-        <v>17</v>
-      </c>
-      <c r="D134" t="s">
-        <v>20</v>
-      </c>
-      <c r="E134" t="s">
-        <v>26</v>
-      </c>
-      <c r="F134" t="s">
-        <v>27</v>
-      </c>
-      <c r="G134" t="s">
-        <v>15</v>
-      </c>
-      <c r="H134" t="s">
-        <v>18</v>
-      </c>
-      <c r="I134" t="s">
-        <v>22</v>
-      </c>
-      <c r="J134" t="s">
-        <v>28</v>
-      </c>
-      <c r="K134" t="s">
-        <v>29</v>
-      </c>
-      <c r="L134" t="s">
-        <v>30</v>
-      </c>
-      <c r="M134" t="s">
-        <v>31</v>
-      </c>
-      <c r="N134" t="s">
-        <v>32</v>
-      </c>
-      <c r="O134" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135" t="s">
+        <v>25</v>
+      </c>
+      <c r="C135" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" t="s">
+        <v>20</v>
+      </c>
+      <c r="E135" t="s">
+        <v>26</v>
+      </c>
+      <c r="F135" t="s">
+        <v>27</v>
+      </c>
+      <c r="G135" t="s">
+        <v>15</v>
+      </c>
+      <c r="H135" t="s">
+        <v>18</v>
+      </c>
+      <c r="I135" t="s">
+        <v>22</v>
+      </c>
+      <c r="J135" t="s">
+        <v>28</v>
+      </c>
+      <c r="K135" t="s">
+        <v>29</v>
+      </c>
+      <c r="L135" t="s">
+        <v>30</v>
+      </c>
+      <c r="M135" t="s">
+        <v>31</v>
+      </c>
+      <c r="N135" t="s">
+        <v>32</v>
+      </c>
+      <c r="O135" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>108</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" t="s">
         <v>107</v>
       </c>
-      <c r="C135">
+      <c r="C136">
         <v>1</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D136" t="s">
         <v>21</v>
       </c>
-      <c r="E135" t="str">
+      <c r="E136" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F135" t="s">
-        <v>34</v>
-      </c>
-      <c r="G135" t="s">
-        <v>16</v>
-      </c>
-      <c r="H135" t="s">
-        <v>35</v>
-      </c>
-      <c r="I135" t="s">
-        <v>54</v>
-      </c>
-      <c r="J135">
-        <v>0</v>
-      </c>
-      <c r="K135" t="s">
-        <v>36</v>
-      </c>
-      <c r="L135" t="s">
-        <v>36</v>
-      </c>
-      <c r="M135" t="s">
-        <v>36</v>
-      </c>
-      <c r="N135" t="s">
-        <v>36</v>
-      </c>
-      <c r="O135" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>36</v>
-      </c>
-      <c r="B136" t="s">
-        <v>69</v>
-      </c>
-      <c r="C136">
-        <v>0.114</v>
-      </c>
-      <c r="D136" t="s">
-        <v>48</v>
-      </c>
-      <c r="E136" t="s">
-        <v>124</v>
-      </c>
       <c r="F136" t="s">
         <v>34</v>
       </c>
@@ -3738,269 +3696,267 @@
         <v>16</v>
       </c>
       <c r="H136" t="s">
+        <v>35</v>
+      </c>
+      <c r="I136" t="s">
+        <v>54</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136" t="s">
+        <v>36</v>
+      </c>
+      <c r="L136" t="s">
+        <v>36</v>
+      </c>
+      <c r="M136" t="s">
+        <v>36</v>
+      </c>
+      <c r="N136" t="s">
+        <v>36</v>
+      </c>
+      <c r="O136" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>36</v>
+      </c>
+      <c r="B137" t="s">
+        <v>69</v>
+      </c>
+      <c r="C137">
+        <v>0.114</v>
+      </c>
+      <c r="D137" t="s">
+        <v>48</v>
+      </c>
+      <c r="E137" t="s">
+        <v>123</v>
+      </c>
+      <c r="F137" t="s">
+        <v>34</v>
+      </c>
+      <c r="G137" t="s">
+        <v>16</v>
+      </c>
+      <c r="H137" t="s">
         <v>42</v>
       </c>
-      <c r="I136" t="s">
+      <c r="I137" t="s">
         <v>70</v>
       </c>
-      <c r="J136">
-        <v>0</v>
-      </c>
-      <c r="K136" t="s">
-        <v>36</v>
-      </c>
-      <c r="L136" t="s">
-        <v>36</v>
-      </c>
-      <c r="M136" t="s">
-        <v>36</v>
-      </c>
-      <c r="N136" t="s">
-        <v>36</v>
-      </c>
-      <c r="O136" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="138" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B138" s="10" t="s">
-        <v>130</v>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137" t="s">
+        <v>36</v>
+      </c>
+      <c r="L137" t="s">
+        <v>36</v>
+      </c>
+      <c r="M137" t="s">
+        <v>36</v>
+      </c>
+      <c r="N137" t="s">
+        <v>36</v>
+      </c>
+      <c r="O137" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="139" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="140" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>15</v>
-      </c>
-      <c r="B141" t="s">
-        <v>101</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>11</v>
-      </c>
-      <c r="B142">
-        <v>102</v>
+        <v>15</v>
+      </c>
+      <c r="B142" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>18</v>
-      </c>
-      <c r="B144" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B145" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B147" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>9</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>25</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>17</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D149" t="s">
         <v>20</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E149" t="s">
         <v>26</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F149" t="s">
         <v>27</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G149" t="s">
         <v>15</v>
       </c>
-      <c r="H148" t="s">
+      <c r="H149" t="s">
         <v>18</v>
       </c>
-      <c r="I148" t="s">
+      <c r="I149" t="s">
         <v>22</v>
       </c>
-      <c r="J148" t="s">
+      <c r="J149" t="s">
         <v>28</v>
       </c>
-      <c r="K148" t="s">
+      <c r="K149" t="s">
         <v>29</v>
       </c>
-      <c r="L148" t="s">
+      <c r="L149" t="s">
         <v>30</v>
       </c>
-      <c r="M148" t="s">
+      <c r="M149" t="s">
         <v>31</v>
       </c>
-      <c r="N148" t="s">
+      <c r="N149" t="s">
         <v>32</v>
       </c>
-      <c r="O148" t="s">
+      <c r="O149" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A149" t="str">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A150" t="str">
+        <f>B140</f>
+        <v>sec_tre__qua_tre</v>
+      </c>
+      <c r="B150" t="str">
         <f>B139</f>
-        <v>ind_ww__dec_tre</v>
-      </c>
-      <c r="B149" t="str">
-        <f>B138</f>
         <v>Ozonation</v>
       </c>
-      <c r="C149">
+      <c r="C150">
         <v>1</v>
       </c>
-      <c r="D149" t="str">
-        <f>B145</f>
+      <c r="D150" t="str">
+        <f>B146</f>
         <v>cubic meter</v>
       </c>
-      <c r="E149" t="str">
+      <c r="E150" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F149" t="s">
+      <c r="F150" t="s">
         <v>34</v>
       </c>
-      <c r="G149" t="str">
-        <f>B141</f>
-        <v>Europe without Switzerland</v>
-      </c>
-      <c r="H149" t="s">
+      <c r="G150" t="str">
+        <f>B142</f>
+        <v>DE</v>
+      </c>
+      <c r="H150" t="s">
         <v>35</v>
       </c>
-      <c r="I149" t="str">
-        <f>B146</f>
+      <c r="I150" t="str">
+        <f>B147</f>
         <v>treated wastewater</v>
       </c>
-      <c r="J149">
-        <v>0</v>
-      </c>
-      <c r="K149" t="s">
-        <v>36</v>
-      </c>
-      <c r="L149" t="s">
-        <v>36</v>
-      </c>
-      <c r="M149" t="s">
-        <v>36</v>
-      </c>
-      <c r="N149" t="s">
-        <v>36</v>
-      </c>
-      <c r="O149" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>36</v>
-      </c>
-      <c r="B150" t="str">
-        <f>B122</f>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150" t="s">
+        <v>36</v>
+      </c>
+      <c r="L150" t="s">
+        <v>36</v>
+      </c>
+      <c r="M150" t="s">
+        <v>36</v>
+      </c>
+      <c r="N150" t="s">
+        <v>36</v>
+      </c>
+      <c r="O150" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>36</v>
+      </c>
+      <c r="B151" t="str">
+        <f>B123</f>
         <v>Chemicals 102</v>
-      </c>
-      <c r="C150">
-        <v>1</v>
-      </c>
-      <c r="D150" t="str">
-        <f>B145</f>
-        <v>cubic meter</v>
-      </c>
-      <c r="E150" t="str">
-        <f>E149</f>
-        <v>paw_db</v>
-      </c>
-      <c r="F150" t="s">
-        <v>41</v>
-      </c>
-      <c r="G150" t="str">
-        <f>B128</f>
-        <v>RER</v>
-      </c>
-      <c r="H150" t="s">
-        <v>42</v>
-      </c>
-      <c r="I150" t="str">
-        <f>B131</f>
-        <v>cubic meter</v>
-      </c>
-      <c r="J150">
-        <v>0</v>
-      </c>
-      <c r="K150" t="s">
-        <v>36</v>
-      </c>
-      <c r="L150" t="s">
-        <v>36</v>
-      </c>
-      <c r="M150" t="s">
-        <v>36</v>
-      </c>
-      <c r="N150" t="s">
-        <v>36</v>
-      </c>
-      <c r="O150" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B151" t="str">
-        <f>B106</f>
-        <v>Electricity 102</v>
       </c>
       <c r="C151">
         <v>1</v>
       </c>
       <c r="D151" t="str">
-        <f>B115</f>
+        <f>B146</f>
         <v>cubic meter</v>
       </c>
       <c r="E151" t="str">
@@ -4008,252 +3964,254 @@
         <v>paw_db</v>
       </c>
       <c r="F151" t="s">
+        <v>41</v>
+      </c>
+      <c r="G151" t="str">
+        <f>B129</f>
+        <v>RER</v>
+      </c>
+      <c r="H151" t="s">
+        <v>42</v>
+      </c>
+      <c r="I151" t="str">
+        <f>B132</f>
+        <v>cubic meter</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151" t="s">
+        <v>36</v>
+      </c>
+      <c r="L151" t="s">
+        <v>36</v>
+      </c>
+      <c r="M151" t="s">
+        <v>36</v>
+      </c>
+      <c r="N151" t="s">
+        <v>36</v>
+      </c>
+      <c r="O151" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B152" t="str">
+        <f>B107</f>
+        <v>Electricity 102</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152" t="str">
+        <f>B116</f>
+        <v>cubic meter</v>
+      </c>
+      <c r="E152" t="str">
+        <f>E151</f>
+        <v>paw_db</v>
+      </c>
+      <c r="F152" t="s">
         <v>34</v>
       </c>
-      <c r="G151" t="str">
-        <f>B115</f>
+      <c r="G152" t="str">
+        <f>B116</f>
         <v>cubic meter</v>
       </c>
-      <c r="H151" t="str">
-        <f>H150</f>
+      <c r="H152" t="str">
+        <f>H151</f>
         <v>technosphere</v>
       </c>
-      <c r="I151" t="str">
-        <f>B115</f>
+      <c r="I152" t="str">
+        <f>B116</f>
         <v>cubic meter</v>
       </c>
-      <c r="J151">
-        <v>0</v>
-      </c>
-      <c r="K151" t="s">
-        <v>36</v>
-      </c>
-      <c r="L151" t="s">
-        <v>36</v>
-      </c>
-      <c r="M151" t="s">
-        <v>36</v>
-      </c>
-      <c r="N151" t="s">
-        <v>36</v>
-      </c>
-      <c r="O151" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="152" spans="1:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B153" s="10" t="s">
-        <v>129</v>
-      </c>
-    </row>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="K152" t="s">
+        <v>36</v>
+      </c>
+      <c r="L152" t="s">
+        <v>36</v>
+      </c>
+      <c r="M152" t="s">
+        <v>36</v>
+      </c>
+      <c r="N152" t="s">
+        <v>36</v>
+      </c>
+      <c r="O152" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="154" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="10" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="155" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>10</v>
-      </c>
-      <c r="B156" t="s">
-        <v>111</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
-      </c>
-      <c r="B157" s="9">
-        <v>128</v>
+        <v>10</v>
+      </c>
+      <c r="B157" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>12</v>
-      </c>
-      <c r="B158" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B158" s="9">
+        <v>128</v>
       </c>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B160" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>17</v>
-      </c>
-      <c r="B161">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B161" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>18</v>
-      </c>
-      <c r="B162" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B163" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B164" t="s">
-        <v>131</v>
+        <v>21</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>9</v>
-      </c>
-      <c r="B166" t="s">
-        <v>25</v>
-      </c>
-      <c r="C166" t="s">
-        <v>17</v>
-      </c>
-      <c r="D166" t="s">
-        <v>20</v>
-      </c>
-      <c r="E166" t="s">
-        <v>26</v>
-      </c>
-      <c r="F166" t="s">
-        <v>27</v>
-      </c>
-      <c r="G166" t="s">
-        <v>15</v>
-      </c>
-      <c r="H166" t="s">
-        <v>18</v>
-      </c>
-      <c r="I166" t="s">
-        <v>22</v>
-      </c>
-      <c r="J166" t="s">
-        <v>28</v>
-      </c>
-      <c r="K166" t="s">
-        <v>29</v>
-      </c>
-      <c r="L166" t="s">
-        <v>30</v>
-      </c>
-      <c r="M166" t="s">
-        <v>31</v>
-      </c>
-      <c r="N166" t="s">
-        <v>32</v>
-      </c>
-      <c r="O166" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" t="s">
+        <v>25</v>
+      </c>
+      <c r="C167" t="s">
+        <v>17</v>
+      </c>
+      <c r="D167" t="s">
+        <v>20</v>
+      </c>
+      <c r="E167" t="s">
+        <v>26</v>
+      </c>
+      <c r="F167" t="s">
+        <v>27</v>
+      </c>
+      <c r="G167" t="s">
+        <v>15</v>
+      </c>
+      <c r="H167" t="s">
+        <v>18</v>
+      </c>
+      <c r="I167" t="s">
+        <v>22</v>
+      </c>
+      <c r="J167" t="s">
+        <v>28</v>
+      </c>
+      <c r="K167" t="s">
+        <v>29</v>
+      </c>
+      <c r="L167" t="s">
+        <v>30</v>
+      </c>
+      <c r="M167" t="s">
+        <v>31</v>
+      </c>
+      <c r="N167" t="s">
+        <v>32</v>
+      </c>
+      <c r="O167" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>110</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>109</v>
       </c>
-      <c r="C167">
+      <c r="C168">
         <v>1</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D168" t="s">
         <v>21</v>
       </c>
-      <c r="E167" t="str">
+      <c r="E168" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F167" t="s">
-        <v>34</v>
-      </c>
-      <c r="G167" t="s">
-        <v>16</v>
-      </c>
-      <c r="H167" t="s">
-        <v>35</v>
-      </c>
-      <c r="I167" t="s">
-        <v>54</v>
-      </c>
-      <c r="J167">
-        <v>0</v>
-      </c>
-      <c r="K167" t="s">
-        <v>36</v>
-      </c>
-      <c r="L167" t="s">
-        <v>36</v>
-      </c>
-      <c r="M167" t="s">
-        <v>36</v>
-      </c>
-      <c r="N167" t="s">
-        <v>36</v>
-      </c>
-      <c r="O167" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>36</v>
-      </c>
-      <c r="B168" t="s">
-        <v>61</v>
-      </c>
-      <c r="C168">
-        <v>0.02</v>
-      </c>
-      <c r="D168" t="s">
-        <v>48</v>
-      </c>
-      <c r="E168" t="s">
-        <v>124</v>
-      </c>
       <c r="F168" t="s">
         <v>34</v>
       </c>
@@ -4261,10 +4219,10 @@
         <v>16</v>
       </c>
       <c r="H168" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="I168" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J168">
         <v>0</v>
@@ -4290,16 +4248,16 @@
         <v>36</v>
       </c>
       <c r="B169" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D169" t="s">
         <v>48</v>
       </c>
       <c r="E169" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F169" t="s">
         <v>34</v>
@@ -4311,7 +4269,7 @@
         <v>42</v>
       </c>
       <c r="I169" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J169">
         <v>0</v>
@@ -4337,16 +4295,16 @@
         <v>36</v>
       </c>
       <c r="B170" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="C170">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="D170" t="s">
         <v>48</v>
       </c>
       <c r="E170" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F170" t="s">
         <v>34</v>
@@ -4358,882 +4316,937 @@
         <v>42</v>
       </c>
       <c r="I170" t="s">
+        <v>60</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+      <c r="K170" t="s">
+        <v>36</v>
+      </c>
+      <c r="L170" t="s">
+        <v>36</v>
+      </c>
+      <c r="M170" t="s">
+        <v>36</v>
+      </c>
+      <c r="N170" t="s">
+        <v>36</v>
+      </c>
+      <c r="O170" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>36</v>
+      </c>
+      <c r="B171" t="s">
+        <v>112</v>
+      </c>
+      <c r="C171">
+        <v>0.02</v>
+      </c>
+      <c r="D171" t="s">
+        <v>48</v>
+      </c>
+      <c r="E171" t="s">
+        <v>123</v>
+      </c>
+      <c r="F171" t="s">
+        <v>34</v>
+      </c>
+      <c r="G171" t="s">
+        <v>16</v>
+      </c>
+      <c r="H171" t="s">
+        <v>42</v>
+      </c>
+      <c r="I171" t="s">
         <v>113</v>
       </c>
-      <c r="J170">
-        <v>0</v>
-      </c>
-      <c r="K170" t="s">
-        <v>36</v>
-      </c>
-      <c r="L170" t="s">
-        <v>36</v>
-      </c>
-      <c r="M170" t="s">
-        <v>36</v>
-      </c>
-      <c r="N170" t="s">
-        <v>36</v>
-      </c>
-      <c r="O170" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="172" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B172" s="10" t="s">
-        <v>114</v>
+      <c r="J171">
+        <v>0</v>
+      </c>
+      <c r="K171" t="s">
+        <v>36</v>
+      </c>
+      <c r="L171" t="s">
+        <v>36</v>
+      </c>
+      <c r="M171" t="s">
+        <v>36</v>
+      </c>
+      <c r="N171" t="s">
+        <v>36</v>
+      </c>
+      <c r="O171" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="173" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="10" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
     </row>
     <row r="174" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>15</v>
-      </c>
-      <c r="B175" t="s">
-        <v>101</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>17</v>
-      </c>
-      <c r="B176">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B176" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>18</v>
-      </c>
-      <c r="B177" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B178" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B179" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B180" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
         <v>9</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" t="s">
         <v>25</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C182" t="s">
         <v>17</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D182" t="s">
         <v>20</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E182" t="s">
         <v>26</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F182" t="s">
         <v>27</v>
       </c>
-      <c r="G181" t="s">
+      <c r="G182" t="s">
         <v>15</v>
       </c>
-      <c r="H181" t="s">
+      <c r="H182" t="s">
         <v>18</v>
       </c>
-      <c r="I181" t="s">
+      <c r="I182" t="s">
         <v>22</v>
       </c>
-      <c r="J181" t="s">
+      <c r="J182" t="s">
         <v>28</v>
       </c>
-      <c r="K181" t="s">
+      <c r="K182" t="s">
         <v>29</v>
       </c>
-      <c r="L181" t="s">
+      <c r="L182" t="s">
         <v>30</v>
       </c>
-      <c r="M181" t="s">
+      <c r="M182" t="s">
         <v>31</v>
       </c>
-      <c r="N181" t="s">
+      <c r="N182" t="s">
         <v>32</v>
       </c>
-      <c r="O181" t="s">
+      <c r="O182" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A182" t="str">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A183" t="str">
+        <f>B174</f>
+        <v>qua_tre__inc</v>
+      </c>
+      <c r="B183" t="str">
         <f>B173</f>
-        <v>qua_tre__inc</v>
-      </c>
-      <c r="B182" t="str">
-        <f>B172</f>
         <v xml:space="preserve">sludge incineration </v>
       </c>
-      <c r="C182">
+      <c r="C183">
         <v>1</v>
       </c>
-      <c r="D182" t="str">
-        <f>B178</f>
+      <c r="D183" t="str">
+        <f>B179</f>
         <v>kilogram</v>
       </c>
-      <c r="E182" t="str">
+      <c r="E183" t="str">
         <f>B2</f>
         <v>paw_db</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F183" t="s">
         <v>34</v>
       </c>
-      <c r="G182" t="str">
-        <f>B175</f>
+      <c r="G183" t="str">
+        <f>B176</f>
         <v>Europe without Switzerland</v>
       </c>
-      <c r="H182" t="s">
+      <c r="H183" t="s">
         <v>35</v>
       </c>
-      <c r="I182" t="str">
-        <f>B179</f>
+      <c r="I183" t="str">
+        <f>B180</f>
         <v>sewage sludge, 70% water, WWT, WW, average</v>
       </c>
-      <c r="J182">
-        <v>0</v>
-      </c>
-      <c r="K182" t="s">
-        <v>36</v>
-      </c>
-      <c r="L182" t="s">
-        <v>36</v>
-      </c>
-      <c r="M182" t="s">
-        <v>36</v>
-      </c>
-      <c r="N182" t="s">
-        <v>36</v>
-      </c>
-      <c r="O182" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>36</v>
-      </c>
-      <c r="B183" t="s">
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="K183" t="s">
+        <v>36</v>
+      </c>
+      <c r="L183" t="s">
+        <v>36</v>
+      </c>
+      <c r="M183" t="s">
+        <v>36</v>
+      </c>
+      <c r="N183" t="s">
+        <v>36</v>
+      </c>
+      <c r="O183" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>36</v>
+      </c>
+      <c r="B184" t="s">
         <v>116</v>
       </c>
-      <c r="C183">
+      <c r="C184">
         <v>1</v>
       </c>
-      <c r="D183" t="str">
-        <f>D182</f>
+      <c r="D184" t="str">
+        <f>D183</f>
         <v>kilogram</v>
       </c>
-      <c r="E183" t="s">
-        <v>124</v>
-      </c>
-      <c r="F183" t="s">
+      <c r="E184" t="s">
+        <v>123</v>
+      </c>
+      <c r="F184" t="s">
         <v>41</v>
       </c>
-      <c r="G183" t="str">
-        <f>B175</f>
+      <c r="G184" t="str">
+        <f>B176</f>
         <v>Europe without Switzerland</v>
       </c>
-      <c r="H183" t="s">
+      <c r="H184" t="s">
         <v>42</v>
       </c>
-      <c r="I183" t="s">
+      <c r="I184" t="s">
         <v>115</v>
       </c>
-      <c r="J183">
-        <v>0</v>
-      </c>
-      <c r="K183" t="s">
-        <v>36</v>
-      </c>
-      <c r="L183" t="s">
-        <v>36</v>
-      </c>
-      <c r="M183" t="s">
-        <v>36</v>
-      </c>
-      <c r="N183" t="s">
-        <v>36</v>
-      </c>
-      <c r="O183" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="184" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B185" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184" t="s">
+        <v>36</v>
+      </c>
+      <c r="L184" t="s">
+        <v>36</v>
+      </c>
+      <c r="M184" t="s">
+        <v>36</v>
+      </c>
+      <c r="N184" t="s">
+        <v>36</v>
+      </c>
+      <c r="O184" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="186" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="10" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="187" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B187" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B187" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>15</v>
-      </c>
-      <c r="B188" t="s">
-        <v>101</v>
+    </row>
+    <row r="188" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B188" s="10" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>17</v>
-      </c>
-      <c r="B189">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B189" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>18</v>
-      </c>
-      <c r="B190" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B191" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B192" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B193" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
         <v>9</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B195" t="s">
         <v>25</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C195" t="s">
         <v>17</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D195" t="s">
         <v>20</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E195" t="s">
         <v>26</v>
       </c>
-      <c r="F194" t="s">
+      <c r="F195" t="s">
         <v>27</v>
       </c>
-      <c r="G194" t="s">
+      <c r="G195" t="s">
         <v>15</v>
       </c>
-      <c r="H194" t="s">
+      <c r="H195" t="s">
         <v>18</v>
       </c>
-      <c r="I194" t="s">
+      <c r="I195" t="s">
         <v>22</v>
       </c>
-      <c r="J194" t="s">
+      <c r="J195" t="s">
         <v>28</v>
       </c>
-      <c r="K194" t="s">
+      <c r="K195" t="s">
         <v>29</v>
       </c>
-      <c r="L194" t="s">
+      <c r="L195" t="s">
         <v>30</v>
       </c>
-      <c r="M194" t="s">
+      <c r="M195" t="s">
         <v>31</v>
       </c>
-      <c r="N194" t="s">
+      <c r="N195" t="s">
         <v>32</v>
       </c>
-      <c r="O194" t="s">
+      <c r="O195" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A195" t="str">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A196" t="str">
+        <f>B187</f>
+        <v>dec_tre__sec_tre</v>
+      </c>
+      <c r="B196" t="str">
         <f>B186</f>
-        <v>dec_tre__sec_tre</v>
-      </c>
-      <c r="B195" t="str">
-        <f>B185</f>
         <v>secondary treatment</v>
       </c>
-      <c r="C195">
+      <c r="C196">
         <v>1</v>
       </c>
-      <c r="D195" t="str">
-        <f>B191</f>
+      <c r="D196" t="str">
+        <f>B192</f>
         <v>cubic meter</v>
       </c>
-      <c r="E195" t="str">
+      <c r="E196" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F195" t="s">
+      <c r="F196" t="s">
         <v>34</v>
       </c>
-      <c r="G195" t="str">
-        <f>B188</f>
+      <c r="G196" t="str">
+        <f>B189</f>
         <v>Europe without Switzerland</v>
       </c>
-      <c r="H195" t="s">
+      <c r="H196" t="s">
         <v>35</v>
       </c>
-      <c r="I195" t="str">
+      <c r="I196" t="str">
+        <f>B193</f>
+        <v>wastewater, average</v>
+      </c>
+      <c r="J196">
+        <v>0</v>
+      </c>
+      <c r="K196" t="s">
+        <v>36</v>
+      </c>
+      <c r="L196" t="s">
+        <v>36</v>
+      </c>
+      <c r="M196" t="s">
+        <v>36</v>
+      </c>
+      <c r="N196" t="s">
+        <v>36</v>
+      </c>
+      <c r="O196" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>36</v>
+      </c>
+      <c r="B197" t="s">
+        <v>95</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197" t="str">
         <f>B192</f>
+        <v>cubic meter</v>
+      </c>
+      <c r="E197" t="s">
+        <v>123</v>
+      </c>
+      <c r="F197" t="s">
+        <v>41</v>
+      </c>
+      <c r="G197" t="str">
+        <f>B189</f>
+        <v>Europe without Switzerland</v>
+      </c>
+      <c r="H197" t="s">
+        <v>42</v>
+      </c>
+      <c r="I197" t="str">
+        <f>B193</f>
         <v>wastewater, average</v>
       </c>
-      <c r="J195">
-        <v>0</v>
-      </c>
-      <c r="K195" t="s">
-        <v>36</v>
-      </c>
-      <c r="L195" t="s">
-        <v>36</v>
-      </c>
-      <c r="M195" t="s">
-        <v>36</v>
-      </c>
-      <c r="N195" t="s">
-        <v>36</v>
-      </c>
-      <c r="O195" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>36</v>
-      </c>
-      <c r="B196" t="s">
-        <v>95</v>
-      </c>
-      <c r="C196">
-        <v>1</v>
-      </c>
-      <c r="D196" t="str">
-        <f>B191</f>
-        <v>cubic meter</v>
-      </c>
-      <c r="E196" t="s">
-        <v>124</v>
-      </c>
-      <c r="F196" t="s">
-        <v>41</v>
-      </c>
-      <c r="G196" t="str">
-        <f>B188</f>
-        <v>Europe without Switzerland</v>
-      </c>
-      <c r="H196" t="s">
-        <v>42</v>
-      </c>
-      <c r="I196" t="str">
-        <f>B192</f>
-        <v>wastewater, average</v>
-      </c>
-      <c r="J196">
-        <v>0</v>
-      </c>
-      <c r="K196" t="s">
-        <v>36</v>
-      </c>
-      <c r="L196" t="s">
-        <v>36</v>
-      </c>
-      <c r="M196" t="s">
-        <v>36</v>
-      </c>
-      <c r="N196" t="s">
-        <v>36</v>
-      </c>
-      <c r="O196" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="198" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B198" s="10" t="s">
-        <v>119</v>
+      <c r="J197">
+        <v>0</v>
+      </c>
+      <c r="K197" t="s">
+        <v>36</v>
+      </c>
+      <c r="L197" t="s">
+        <v>36</v>
+      </c>
+      <c r="M197" t="s">
+        <v>36</v>
+      </c>
+      <c r="N197" t="s">
+        <v>36</v>
+      </c>
+      <c r="O197" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="199" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B199" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>15</v>
-      </c>
-      <c r="B200" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>17</v>
-      </c>
-      <c r="B201">
-        <v>1</v>
+      <c r="B200" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B202" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>20</v>
-      </c>
-      <c r="B203" t="s">
-        <v>126</v>
+        <v>17</v>
+      </c>
+      <c r="B203">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B204" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B205" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>22</v>
+      </c>
+      <c r="B206" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
         <v>9</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B208" t="s">
         <v>25</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C208" t="s">
         <v>17</v>
       </c>
-      <c r="D206" t="s">
+      <c r="D208" t="s">
         <v>20</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E208" t="s">
         <v>26</v>
       </c>
-      <c r="F206" t="s">
+      <c r="F208" t="s">
         <v>27</v>
       </c>
-      <c r="G206" t="s">
+      <c r="G208" t="s">
         <v>15</v>
       </c>
-      <c r="H206" t="s">
+      <c r="H208" t="s">
         <v>18</v>
       </c>
-      <c r="I206" t="s">
+      <c r="I208" t="s">
         <v>22</v>
       </c>
-      <c r="J206" t="s">
+      <c r="J208" t="s">
         <v>28</v>
       </c>
-      <c r="K206" t="s">
+      <c r="K208" t="s">
         <v>29</v>
       </c>
-      <c r="L206" t="s">
+      <c r="L208" t="s">
         <v>30</v>
       </c>
-      <c r="M206" t="s">
+      <c r="M208" t="s">
         <v>31</v>
       </c>
-      <c r="N206" t="s">
+      <c r="N208" t="s">
         <v>32</v>
       </c>
-      <c r="O206" t="s">
+      <c r="O208" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A207" t="str">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A209" t="str">
+        <f>B200</f>
+        <v>sldg_sep__inc</v>
+      </c>
+      <c r="B209" t="str">
         <f>B199</f>
-        <v>sldg_sep__inc</v>
-      </c>
-      <c r="B207" t="str">
-        <f>B198</f>
         <v>transport of sludge to incineration</v>
       </c>
-      <c r="C207">
+      <c r="C209">
         <v>1</v>
       </c>
-      <c r="D207" t="str">
-        <f>B203</f>
+      <c r="D209" t="str">
+        <f>B205</f>
         <v>ton kilometer</v>
       </c>
-      <c r="E207" t="str">
+      <c r="E209" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F207" t="s">
+      <c r="F209" t="s">
         <v>34</v>
       </c>
-      <c r="G207" t="str">
-        <f>B200</f>
+      <c r="G209" t="str">
+        <f>B202</f>
         <v>RER</v>
       </c>
-      <c r="H207" t="s">
+      <c r="H209" t="s">
         <v>35</v>
       </c>
-      <c r="I207" t="str">
-        <f>B204</f>
+      <c r="I209" t="str">
+        <f>B206</f>
         <v>transport, freight, lorry, diesel, unspecified</v>
       </c>
-      <c r="J207">
-        <v>0</v>
-      </c>
-      <c r="K207" t="s">
-        <v>36</v>
-      </c>
-      <c r="L207" t="s">
-        <v>36</v>
-      </c>
-      <c r="M207" t="s">
-        <v>36</v>
-      </c>
-      <c r="N207" t="s">
-        <v>36</v>
-      </c>
-      <c r="O207" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>36</v>
-      </c>
-      <c r="B208" t="s">
-        <v>122</v>
-      </c>
-      <c r="C208">
+      <c r="J209">
+        <v>0</v>
+      </c>
+      <c r="K209" t="s">
+        <v>36</v>
+      </c>
+      <c r="L209" t="s">
+        <v>36</v>
+      </c>
+      <c r="M209" t="s">
+        <v>36</v>
+      </c>
+      <c r="N209" t="s">
+        <v>36</v>
+      </c>
+      <c r="O209" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>36</v>
+      </c>
+      <c r="B210" t="s">
+        <v>121</v>
+      </c>
+      <c r="C210">
         <v>100</v>
       </c>
-      <c r="D208" t="str">
-        <f>B203</f>
+      <c r="D210" t="str">
+        <f>B205</f>
         <v>ton kilometer</v>
       </c>
-      <c r="E208" t="s">
-        <v>124</v>
-      </c>
-      <c r="F208" t="s">
+      <c r="E210" t="s">
+        <v>123</v>
+      </c>
+      <c r="F210" t="s">
         <v>41</v>
       </c>
-      <c r="G208" t="str">
-        <f>B200</f>
+      <c r="G210" t="str">
+        <f>B202</f>
         <v>RER</v>
       </c>
-      <c r="H208" t="s">
+      <c r="H210" t="s">
         <v>42</v>
       </c>
-      <c r="I208" t="s">
+      <c r="I210" t="s">
+        <v>119</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
+      </c>
+      <c r="K210" t="s">
+        <v>36</v>
+      </c>
+      <c r="L210" t="s">
+        <v>36</v>
+      </c>
+      <c r="M210" t="s">
+        <v>36</v>
+      </c>
+      <c r="N210" t="s">
+        <v>36</v>
+      </c>
+      <c r="O210" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B212" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="J208">
-        <v>0</v>
-      </c>
-      <c r="K208" t="s">
-        <v>36</v>
-      </c>
-      <c r="L208" t="s">
-        <v>36</v>
-      </c>
-      <c r="M208" t="s">
-        <v>36</v>
-      </c>
-      <c r="N208" t="s">
-        <v>36</v>
-      </c>
-      <c r="O208" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B210" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="211" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="10" t="s">
+    </row>
+    <row r="213" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B211" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A212" t="s">
-        <v>15</v>
-      </c>
-      <c r="B212" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>17</v>
-      </c>
-      <c r="B213">
-        <v>1</v>
+      <c r="B213" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B214" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>20</v>
-      </c>
-      <c r="B215" t="s">
-        <v>126</v>
+        <v>17</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B216" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
     </row>
     <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="B217" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>22</v>
+      </c>
+      <c r="B218" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
         <v>9</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B220" t="s">
         <v>25</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C220" t="s">
         <v>17</v>
       </c>
-      <c r="D218" t="s">
+      <c r="D220" t="s">
         <v>20</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E220" t="s">
         <v>26</v>
       </c>
-      <c r="F218" t="s">
+      <c r="F220" t="s">
         <v>27</v>
       </c>
-      <c r="G218" t="s">
+      <c r="G220" t="s">
         <v>15</v>
       </c>
-      <c r="H218" t="s">
+      <c r="H220" t="s">
         <v>18</v>
       </c>
-      <c r="I218" t="s">
+      <c r="I220" t="s">
         <v>22</v>
       </c>
-      <c r="J218" t="s">
+      <c r="J220" t="s">
         <v>28</v>
       </c>
-      <c r="K218" t="s">
+      <c r="K220" t="s">
         <v>29</v>
       </c>
-      <c r="L218" t="s">
+      <c r="L220" t="s">
         <v>30</v>
       </c>
-      <c r="M218" t="s">
+      <c r="M220" t="s">
         <v>31</v>
       </c>
-      <c r="N218" t="s">
+      <c r="N220" t="s">
         <v>32</v>
       </c>
-      <c r="O218" t="s">
+      <c r="O220" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A219" t="str">
-        <f>B211</f>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A221" t="str">
+        <f>B213</f>
         <v>fer__soi</v>
       </c>
-      <c r="B219" t="str">
-        <f>B210</f>
+      <c r="B221" t="str">
+        <f>B212</f>
         <v>transport of fertilizer to soil</v>
       </c>
-      <c r="C219">
+      <c r="C221">
         <v>1</v>
       </c>
-      <c r="D219" t="str">
-        <f>B215</f>
+      <c r="D221" t="str">
+        <f>B217</f>
         <v>ton kilometer</v>
       </c>
-      <c r="E219" t="str">
+      <c r="E221" t="str">
         <f>$B$2</f>
         <v>paw_db</v>
       </c>
-      <c r="F219" t="s">
+      <c r="F221" t="s">
         <v>34</v>
       </c>
-      <c r="G219" t="str">
-        <f>B212</f>
+      <c r="G221" t="str">
+        <f>B214</f>
         <v>RER</v>
       </c>
-      <c r="H219" t="s">
+      <c r="H221" t="s">
         <v>35</v>
       </c>
-      <c r="I219" t="str">
-        <f>B216</f>
+      <c r="I221" t="str">
+        <f>B218</f>
         <v>transport, freight, lorry, diesel, unspecified</v>
       </c>
-      <c r="J219">
-        <v>0</v>
-      </c>
-      <c r="K219" t="s">
-        <v>36</v>
-      </c>
-      <c r="L219" t="s">
-        <v>36</v>
-      </c>
-      <c r="M219" t="s">
-        <v>36</v>
-      </c>
-      <c r="N219" t="s">
-        <v>36</v>
-      </c>
-      <c r="O219" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>36</v>
-      </c>
-      <c r="B220" t="s">
-        <v>122</v>
-      </c>
-      <c r="C220">
+      <c r="J221">
+        <v>0</v>
+      </c>
+      <c r="K221" t="s">
+        <v>36</v>
+      </c>
+      <c r="L221" t="s">
+        <v>36</v>
+      </c>
+      <c r="M221" t="s">
+        <v>36</v>
+      </c>
+      <c r="N221" t="s">
+        <v>36</v>
+      </c>
+      <c r="O221" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>36</v>
+      </c>
+      <c r="B222" t="s">
+        <v>121</v>
+      </c>
+      <c r="C222">
         <v>20</v>
       </c>
-      <c r="D220" t="str">
-        <f>B215</f>
+      <c r="D222" t="str">
+        <f>B217</f>
         <v>ton kilometer</v>
       </c>
-      <c r="E220" t="s">
-        <v>124</v>
-      </c>
-      <c r="F220" t="s">
+      <c r="E222" t="s">
+        <v>123</v>
+      </c>
+      <c r="F222" t="s">
         <v>41</v>
       </c>
-      <c r="G220" t="str">
-        <f>B212</f>
+      <c r="G222" t="str">
+        <f>B214</f>
         <v>RER</v>
       </c>
-      <c r="H220" t="s">
+      <c r="H222" t="s">
         <v>42</v>
       </c>
-      <c r="I220" t="s">
-        <v>120</v>
-      </c>
-      <c r="J220">
-        <v>0</v>
-      </c>
-      <c r="K220" t="s">
-        <v>36</v>
-      </c>
-      <c r="L220" t="s">
-        <v>36</v>
-      </c>
-      <c r="M220" t="s">
-        <v>36</v>
-      </c>
-      <c r="N220" t="s">
-        <v>36</v>
-      </c>
-      <c r="O220" t="s">
+      <c r="I222" t="s">
+        <v>119</v>
+      </c>
+      <c r="J222">
+        <v>0</v>
+      </c>
+      <c r="K222" t="s">
+        <v>36</v>
+      </c>
+      <c r="L222" t="s">
+        <v>36</v>
+      </c>
+      <c r="M222" t="s">
+        <v>36</v>
+      </c>
+      <c r="N222" t="s">
+        <v>36</v>
+      </c>
+      <c r="O222" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change code1 in inventory
</commit_message>
<xml_diff>
--- a/LCA/LCI_ Inventories.xlsx
+++ b/LCA/LCI_ Inventories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welkerm\cursor\PAW_MFA_LCA_2025\LCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\repositories\PAW_MFA_LCA_2025\LCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5AC587-669D-4D85-9D33-645B4FCFB429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9171F6-1887-4FA1-B13E-31491570E266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1500" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EF6BAC2F-8532-4D6B-ADAB-847A45F05723}"/>
   </bookViews>
   <sheets>
     <sheet name="Directory" sheetId="2" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="165">
   <si>
     <t>Database</t>
   </si>
@@ -518,13 +529,16 @@
   </si>
   <si>
     <t>wtr_dis =&gt; irr__cec</t>
+  </si>
+  <si>
+    <t>code1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,7 +644,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -968,14 +982,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>230</v>
       </c>
@@ -983,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>102</v>
       </c>
@@ -991,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>128</v>
       </c>
@@ -1008,19 +1022,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9BD897-F590-4437-A121-ED2632AD5485}">
   <dimension ref="A1:O257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" zoomScale="173" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B241" sqref="B241"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A255" sqref="A255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="8" max="8" width="15.125" customWidth="1"/>
-    <col min="9" max="9" width="21.125" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" ht="15">
+    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1050,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1074,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1090,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1084,7 +1098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1108,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1116,7 +1130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1124,7 +1138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1132,12 +1146,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1232,7 +1246,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1279,7 +1293,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1303,7 +1317,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1319,7 +1333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1335,7 +1349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1343,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1351,7 +1365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1359,7 +1373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1367,12 +1381,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1467,7 +1481,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1514,7 +1528,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1561,7 +1575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
@@ -1569,7 +1583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1577,7 +1591,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -1593,7 +1607,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1601,7 +1615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1617,7 +1631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1625,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +1647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -1641,7 +1655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>22</v>
       </c>
@@ -1649,12 +1663,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1701,7 +1715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1749,7 +1763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -1796,7 +1810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1843,7 +1857,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1890,7 +1904,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1937,7 +1951,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1984,7 +1998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -2031,7 +2045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2078,7 +2092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -2125,7 +2139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -2172,7 +2186,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -2219,7 +2233,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -2266,7 +2280,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -2313,7 +2327,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -2360,7 +2374,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -2407,7 +2421,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -2454,7 +2468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -2501,7 +2515,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -2548,7 +2562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -2595,7 +2609,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -2603,7 +2617,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>9</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -2619,7 +2633,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -2627,7 +2641,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -2635,7 +2649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>14</v>
       </c>
@@ -2643,7 +2657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -2651,7 +2665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -2659,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -2667,7 +2681,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>20</v>
       </c>
@@ -2675,7 +2689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -2683,12 +2697,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -2735,7 +2749,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -2783,7 +2797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -2830,7 +2844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>36</v>
       </c>
@@ -2877,7 +2891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>36</v>
       </c>
@@ -2924,7 +2938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -2971,7 +2985,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>8</v>
       </c>
@@ -2979,15 +2993,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>130</v>
       </c>
@@ -2995,7 +3009,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -3003,7 +3017,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -3011,7 +3025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -3019,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -3027,7 +3041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>20</v>
       </c>
@@ -3035,7 +3049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -3043,12 +3057,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -3095,7 +3109,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="str">
         <f>B91</f>
         <v>sec_tre =&gt; qua_tre__gac</v>
@@ -3148,7 +3162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>36</v>
       </c>
@@ -3200,7 +3214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -3252,7 +3266,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>36</v>
       </c>
@@ -3304,7 +3318,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>36</v>
       </c>
@@ -3356,7 +3370,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>8</v>
       </c>
@@ -3364,7 +3378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -3372,7 +3386,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -3380,7 +3394,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -3388,7 +3402,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -3396,7 +3410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -3404,7 +3418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -3412,7 +3426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -3420,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -3428,7 +3442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>20</v>
       </c>
@@ -3436,7 +3450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -3444,12 +3458,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3496,7 +3510,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>105</v>
       </c>
@@ -3544,7 +3558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>36</v>
       </c>
@@ -3591,7 +3605,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>8</v>
       </c>
@@ -3599,7 +3613,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -3607,7 +3621,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -3623,7 +3637,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -3631,7 +3645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>14</v>
       </c>
@@ -3639,7 +3653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>15</v>
       </c>
@@ -3647,7 +3661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>17</v>
       </c>
@@ -3655,7 +3669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -3663,7 +3677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -3671,7 +3685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>22</v>
       </c>
@@ -3679,12 +3693,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +3745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>108</v>
       </c>
@@ -3779,7 +3793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>36</v>
       </c>
@@ -3826,7 +3840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="10" customFormat="1">
+    <row r="139" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="10" t="s">
         <v>8</v>
       </c>
@@ -3834,15 +3848,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="140" spans="1:15" s="10" customFormat="1">
+    <row r="140" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B140" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:15" s="10" customFormat="1">
+    <row r="141" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="10" t="s">
         <v>130</v>
       </c>
@@ -3850,7 +3864,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>15</v>
       </c>
@@ -3858,7 +3872,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -3866,7 +3880,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>17</v>
       </c>
@@ -3874,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>18</v>
       </c>
@@ -3882,7 +3896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>20</v>
       </c>
@@ -3890,7 +3904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>22</v>
       </c>
@@ -3898,12 +3912,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -3950,7 +3964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="str">
         <f>B140</f>
         <v>sec_tre =&gt; qua_tre__o3</v>
@@ -4003,7 +4017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>36</v>
       </c>
@@ -4055,7 +4069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -4108,8 +4122,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="13.7" customHeight="1"/>
-    <row r="154" spans="1:15" s="10" customFormat="1">
+    <row r="153" spans="1:15" ht="13.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="10" t="s">
         <v>8</v>
       </c>
@@ -4117,15 +4131,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="155" spans="1:15" s="10" customFormat="1">
+    <row r="155" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B155" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="156" spans="1:15" s="10" customFormat="1">
+    <row r="156" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="10" t="s">
         <v>130</v>
       </c>
@@ -4133,7 +4147,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -4141,7 +4155,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -4149,7 +4163,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>12</v>
       </c>
@@ -4157,7 +4171,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>14</v>
       </c>
@@ -4165,7 +4179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>15</v>
       </c>
@@ -4173,7 +4187,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>17</v>
       </c>
@@ -4181,7 +4195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>18</v>
       </c>
@@ -4189,7 +4203,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>20</v>
       </c>
@@ -4197,7 +4211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>22</v>
       </c>
@@ -4205,12 +4219,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -4257,7 +4271,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="str">
         <f>B155</f>
         <v>sec_tre =&gt; qua_tre__aop</v>
@@ -4308,7 +4322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -4355,7 +4369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -4402,7 +4416,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -4449,7 +4463,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:15" s="10" customFormat="1">
+    <row r="173" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>8</v>
       </c>
@@ -4457,15 +4471,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="174" spans="1:15" s="10" customFormat="1">
+    <row r="174" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B174" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="175" spans="1:15" s="10" customFormat="1">
+    <row r="175" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="10" t="s">
         <v>130</v>
       </c>
@@ -4473,7 +4487,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="176" spans="1:15" s="10" customFormat="1">
+    <row r="176" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
         <v>149</v>
       </c>
@@ -4481,7 +4495,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="177" spans="1:15" s="10" customFormat="1">
+    <row r="177" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="10" t="s">
         <v>150</v>
       </c>
@@ -4489,7 +4503,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="178" spans="1:15" s="10" customFormat="1">
+    <row r="178" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="10" t="s">
         <v>156</v>
       </c>
@@ -4497,7 +4511,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>15</v>
       </c>
@@ -4505,7 +4519,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>17</v>
       </c>
@@ -4513,7 +4527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>18</v>
       </c>
@@ -4521,7 +4535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>20</v>
       </c>
@@ -4529,7 +4543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>22</v>
       </c>
@@ -4537,12 +4551,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -4589,7 +4603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="str">
         <f>B174</f>
         <v>qua_tre =&gt; inc__nof</v>
@@ -4642,7 +4656,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>36</v>
       </c>
@@ -4691,8 +4705,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15.6" customHeight="1"/>
-    <row r="189" spans="1:15" s="10" customFormat="1">
+    <row r="188" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="10" t="s">
         <v>8</v>
       </c>
@@ -4700,15 +4714,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="190" spans="1:15" s="10" customFormat="1">
+    <row r="190" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B190" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="191" spans="1:15" s="10" customFormat="1">
+    <row r="191" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
         <v>130</v>
       </c>
@@ -4716,7 +4730,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="192" spans="1:15" s="10" customFormat="1">
+    <row r="192" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="10" t="s">
         <v>149</v>
       </c>
@@ -4724,7 +4738,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="10" customFormat="1">
+    <row r="193" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="10" t="s">
         <v>150</v>
       </c>
@@ -4732,7 +4746,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="194" spans="1:15" s="10" customFormat="1">
+    <row r="194" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="10" t="s">
         <v>156</v>
       </c>
@@ -4740,7 +4754,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>15</v>
       </c>
@@ -4748,7 +4762,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>17</v>
       </c>
@@ -4756,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>18</v>
       </c>
@@ -4764,7 +4778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>20</v>
       </c>
@@ -4772,7 +4786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>22</v>
       </c>
@@ -4780,12 +4794,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -4832,7 +4846,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" t="str">
         <f>B192</f>
         <v>dec_tre =&gt; sec_tre__o3</v>
@@ -4885,7 +4899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>36</v>
       </c>
@@ -4935,7 +4949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="205" spans="1:15" s="10" customFormat="1">
+    <row r="205" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="10" t="s">
         <v>8</v>
       </c>
@@ -4943,7 +4957,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="206" spans="1:15" s="10" customFormat="1">
+    <row r="206" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="10" t="s">
         <v>158</v>
       </c>
@@ -4951,7 +4965,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="207" spans="1:15" s="10" customFormat="1">
+    <row r="207" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="10" t="s">
         <v>130</v>
       </c>
@@ -4959,7 +4973,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="208" spans="1:15" s="10" customFormat="1">
+    <row r="208" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="10" t="s">
         <v>149</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="209" spans="1:15" s="10" customFormat="1">
+    <row r="209" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="10" t="s">
         <v>150</v>
       </c>
@@ -4975,7 +4989,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="210" spans="1:15" s="10" customFormat="1">
+    <row r="210" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="10" t="s">
         <v>156</v>
       </c>
@@ -4983,15 +4997,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="211" spans="1:15" s="10" customFormat="1">
+    <row r="211" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B211" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>15</v>
       </c>
@@ -4999,7 +5013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>17</v>
       </c>
@@ -5007,7 +5021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>18</v>
       </c>
@@ -5015,7 +5029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>20</v>
       </c>
@@ -5023,7 +5037,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>22</v>
       </c>
@@ -5031,12 +5045,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -5083,7 +5097,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A219" t="str">
         <f>B211</f>
         <v>sldg_trans</v>
@@ -5136,7 +5150,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>36</v>
       </c>
@@ -5185,7 +5199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="222" spans="1:15" s="10" customFormat="1">
+    <row r="222" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="10" t="s">
         <v>8</v>
       </c>
@@ -5193,15 +5207,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="223" spans="1:15" s="10" customFormat="1">
+    <row r="223" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B223" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>15</v>
       </c>
@@ -5209,7 +5223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>17</v>
       </c>
@@ -5217,7 +5231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>18</v>
       </c>
@@ -5225,7 +5239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>20</v>
       </c>
@@ -5233,7 +5247,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>22</v>
       </c>
@@ -5241,12 +5255,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -5293,7 +5307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A231" t="str">
         <f>B223</f>
         <v>fer =&gt; soi</v>
@@ -5346,7 +5360,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>36</v>
       </c>
@@ -5395,7 +5409,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A234" s="10" t="s">
         <v>8</v>
       </c>
@@ -5403,7 +5417,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A235" s="10" t="s">
         <v>130</v>
       </c>
@@ -5411,15 +5425,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A236" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B236" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>15</v>
       </c>
@@ -5427,7 +5441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:15">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>17</v>
       </c>
@@ -5435,7 +5449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>18</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:15">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>20</v>
       </c>
@@ -5451,7 +5465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>22</v>
       </c>
@@ -5459,12 +5473,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="242" spans="1:15">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -5511,7 +5525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="244" spans="1:15">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>132</v>
       </c>
@@ -5560,7 +5574,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B245" t="s">
         <v>134</v>
       </c>
@@ -5580,7 +5594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A247" s="10" t="s">
         <v>8</v>
       </c>
@@ -5588,15 +5602,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="248" spans="1:15">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A248" s="10" t="s">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="B248" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>15</v>
       </c>
@@ -5604,7 +5618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="250" spans="1:15">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>17</v>
       </c>
@@ -5612,7 +5626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>18</v>
       </c>
@@ -5620,7 +5634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="252" spans="1:15">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>20</v>
       </c>
@@ -5628,7 +5642,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>22</v>
       </c>
@@ -5636,12 +5650,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="254" spans="1:15">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>9</v>
       </c>
@@ -5688,7 +5702,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="256" spans="1:15">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>132</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="257" spans="2:8">
+    <row r="257" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B257" t="s">
         <v>134</v>
       </c>

</xml_diff>